<commit_message>
Deployed fef2dc6 with MkDocs version: 1.3.1
</commit_message>
<xml_diff>
--- a/python/DataStructure/assets/tmp.xlsx
+++ b/python/DataStructure/assets/tmp.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\I310913\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/james/myMemo/mySite/docs/python/DataStructure/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB200FBD-8A00-41B6-9C2C-1B1415C74984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202C0F80-3065-FA47-B576-0243FC0C6359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="2" xr2:uid="{BF1997EC-B4F8-2449-844A-09537E8310CE}"/>
+    <workbookView xWindow="12800" yWindow="760" windowWidth="19380" windowHeight="18880" activeTab="2" xr2:uid="{BF1997EC-B4F8-2449-844A-09537E8310CE}"/>
   </bookViews>
   <sheets>
     <sheet name="算法复杂度" sheetId="1" r:id="rId1"/>
@@ -1597,7 +1597,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1830,12 +1830,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1859,6 +1853,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2339,14 +2339,14 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="5" width="18.33203125" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="7" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="22" customHeight="1">
+    <row r="2" spans="2:7" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="21" customHeight="1">
+    <row r="3" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="21" customHeight="1">
+    <row r="4" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
@@ -2406,7 +2406,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="21" customHeight="1">
+    <row r="5" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
@@ -2426,7 +2426,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="21" customHeight="1">
+    <row r="6" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="21" customHeight="1">
+    <row r="7" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="21" customHeight="1">
+    <row r="8" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="21" customHeight="1">
+    <row r="9" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="21" customHeight="1">
+    <row r="10" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
@@ -2526,7 +2526,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="21" customHeight="1">
+    <row r="11" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="21" customHeight="1">
+    <row r="12" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="7" t="s">
         <v>10</v>
       </c>
@@ -2566,15 +2566,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="36" customHeight="1">
-      <c r="B14" s="12" t="s">
+    <row r="14" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2595,7 +2595,7 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.5" customWidth="1"/>
     <col min="2" max="2" width="62.83203125" style="10" bestFit="1" customWidth="1"/>
@@ -2603,7 +2603,7 @@
     <col min="4" max="4" width="10.83203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" s="5" t="s">
         <v>68</v>
       </c>
@@ -2614,7 +2614,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="s">
         <v>65</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
         <v>63</v>
       </c>
@@ -2636,7 +2636,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:4">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" s="5" t="s">
         <v>61</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
         <v>59</v>
       </c>
@@ -2658,7 +2658,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="2:4">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" s="5" t="s">
         <v>58</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:4">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" s="5" t="s">
         <v>48</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="2:4">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" s="5" t="s">
         <v>52</v>
       </c>
@@ -2691,7 +2691,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:4">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" s="5" t="s">
         <v>50</v>
       </c>
@@ -2702,7 +2702,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" s="5" t="s">
         <v>48</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" s="5" t="s">
         <v>52</v>
       </c>
@@ -2724,7 +2724,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B13" s="5" t="s">
         <v>50</v>
       </c>
@@ -2735,7 +2735,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="2:4">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B14" s="5" t="s">
         <v>48</v>
       </c>
@@ -2746,7 +2746,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="2:4">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
         <v>47</v>
       </c>
@@ -2757,7 +2757,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="2:4">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>45</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
         <v>43</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
         <v>41</v>
       </c>
@@ -2790,14 +2790,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="2:4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="5"/>
       <c r="C19" s="5" t="s">
         <v>39</v>
       </c>
       <c r="D19" s="5"/>
     </row>
-    <row r="20" spans="2:4">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="5"/>
       <c r="C20" s="5" t="s">
         <v>38</v>
@@ -2806,7 +2806,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="2:4">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="5" t="s">
         <v>37</v>
       </c>
@@ -2815,14 +2815,14 @@
       </c>
       <c r="D21" s="5"/>
     </row>
-    <row r="22" spans="2:4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" s="5"/>
       <c r="C22" s="5">
         <v>13</v>
       </c>
       <c r="D22" s="5"/>
     </row>
-    <row r="23" spans="2:4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
         <v>26</v>
       </c>
@@ -2833,7 +2833,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="2:4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="s">
         <v>26</v>
       </c>
@@ -2842,7 +2842,7 @@
       </c>
       <c r="D24" s="5"/>
     </row>
-    <row r="25" spans="2:4">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="s">
         <v>34</v>
       </c>
@@ -2853,21 +2853,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="2:4">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="5"/>
       <c r="C26" s="5" t="s">
         <v>32</v>
       </c>
       <c r="D26" s="5"/>
     </row>
-    <row r="27" spans="2:4">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" s="5"/>
       <c r="C27" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D27" s="5"/>
     </row>
-    <row r="28" spans="2:4">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="5"/>
       <c r="C28" s="5" t="s">
         <v>30</v>
@@ -2876,21 +2876,21 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="2:4">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" s="5"/>
       <c r="C29" s="5" t="s">
         <v>29</v>
       </c>
       <c r="D29" s="5"/>
     </row>
-    <row r="30" spans="2:4">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" s="5"/>
       <c r="C30" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D30" s="5"/>
     </row>
-    <row r="31" spans="2:4">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B31" s="5"/>
       <c r="C31" s="5" t="s">
         <v>27</v>
@@ -2899,7 +2899,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="2:4">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B32" s="5" t="s">
         <v>26</v>
       </c>
@@ -2908,7 +2908,7 @@
       </c>
       <c r="D32" s="5"/>
     </row>
-    <row r="33" spans="2:4">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="5" t="s">
         <v>26</v>
       </c>
@@ -2930,67 +2930,66 @@
       <selection activeCell="AB36" sqref="AB36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="4.33203125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="4.4140625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="2.25" style="10" customWidth="1"/>
-    <col min="5" max="5" width="9.58203125" style="16" customWidth="1"/>
+    <col min="1" max="3" width="4.33203125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="2.1640625" style="10" customWidth="1"/>
+    <col min="5" max="5" width="9.5" style="14" customWidth="1"/>
     <col min="6" max="25" width="4.33203125" style="10" customWidth="1"/>
     <col min="26" max="16384" width="10.83203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:25">
+    <row r="2" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C2" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="19" t="s">
+      <c r="E2" s="15"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
-      <c r="Q2" s="20" t="s">
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="Q2" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
-      <c r="U2" s="21"/>
-      <c r="V2" s="21"/>
-      <c r="W2" s="21"/>
-      <c r="X2" s="21"/>
-      <c r="Y2" s="21"/>
-    </row>
-    <row r="3" spans="3:25">
-      <c r="E3" s="15"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-    </row>
-    <row r="4" spans="3:25">
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="19"/>
+      <c r="Y2" s="19"/>
+    </row>
+    <row r="3" spans="3:25" x14ac:dyDescent="0.2">
+      <c r="E3" s="13"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+    </row>
+    <row r="4" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C4" s="10">
         <v>1</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="14"/>
+      <c r="F4" s="12"/>
       <c r="G4" s="11">
         <v>12</v>
       </c>
@@ -3018,7 +3017,7 @@
       <c r="O4" s="11">
         <v>16</v>
       </c>
-      <c r="P4" s="14"/>
+      <c r="P4" s="12"/>
       <c r="Q4" s="5" t="s">
         <v>69</v>
       </c>
@@ -3047,45 +3046,45 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="3:25">
-      <c r="E5" s="15"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14" t="s">
+    <row r="5" spans="3:25" x14ac:dyDescent="0.2">
+      <c r="E5" s="13"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14" t="s">
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14" t="s">
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="P5" s="14"/>
-    </row>
-    <row r="6" spans="3:25">
-      <c r="E6" s="15"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-    </row>
-    <row r="7" spans="3:25">
+      <c r="P5" s="12"/>
+    </row>
+    <row r="6" spans="3:25" x14ac:dyDescent="0.2">
+      <c r="E6" s="13"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+    </row>
+    <row r="7" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C7" s="10">
         <v>2</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="14" t="s">
         <v>74</v>
       </c>
       <c r="G7" s="11">
@@ -3103,11 +3102,11 @@
       <c r="K7" s="11">
         <v>14</v>
       </c>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
       <c r="Q7" s="5" t="s">
         <v>69</v>
       </c>
@@ -3136,45 +3135,45 @@
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="3:25">
-      <c r="E8" s="15"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14" t="s">
+    <row r="8" spans="3:25" x14ac:dyDescent="0.2">
+      <c r="E8" s="13"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14" t="s">
+      <c r="H8" s="12"/>
+      <c r="I8" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14" t="s">
+      <c r="J8" s="12"/>
+      <c r="K8" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-    </row>
-    <row r="9" spans="3:25">
-      <c r="E9" s="15"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-    </row>
-    <row r="10" spans="3:25">
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+    </row>
+    <row r="9" spans="3:25" x14ac:dyDescent="0.2">
+      <c r="E9" s="13"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+    </row>
+    <row r="10" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C10" s="10">
         <v>3</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="E10" s="14" t="s">
         <v>74</v>
       </c>
       <c r="G10" s="11">
@@ -3186,13 +3185,13 @@
       <c r="I10" s="11">
         <v>17</v>
       </c>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
-      <c r="P10" s="14"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
       <c r="Q10" s="5" t="s">
         <v>69</v>
       </c>
@@ -3221,7 +3220,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" spans="3:25">
+    <row r="11" spans="3:25" x14ac:dyDescent="0.2">
       <c r="G11" s="10" t="s">
         <v>70</v>
       </c>
@@ -3232,25 +3231,25 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="3:25">
-      <c r="E12" s="15"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
-      <c r="P12" s="14"/>
-    </row>
-    <row r="13" spans="3:25">
+    <row r="12" spans="3:25" x14ac:dyDescent="0.2">
+      <c r="E12" s="13"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+    </row>
+    <row r="13" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C13" s="10">
         <v>4</v>
       </c>
-      <c r="E13" s="16" t="s">
+      <c r="E13" s="14" t="s">
         <v>74</v>
       </c>
       <c r="G13" s="11">
@@ -3259,14 +3258,14 @@
       <c r="H13" s="11">
         <v>19</v>
       </c>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
-      <c r="P13" s="14"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
       <c r="Q13" s="5" t="s">
         <v>69</v>
       </c>
@@ -3295,29 +3294,29 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="3:25">
-      <c r="E14" s="15"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14" t="s">
+    <row r="14" spans="3:25" x14ac:dyDescent="0.2">
+      <c r="E14" s="13"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="H14" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-    </row>
-    <row r="16" spans="3:25">
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+    </row>
+    <row r="16" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C16" s="10">
         <v>5</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="14" t="s">
         <v>75</v>
       </c>
       <c r="Q16" s="5">
@@ -3348,38 +3347,38 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="3:25">
-      <c r="E17" s="15"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
-    </row>
-    <row r="18" spans="3:25">
+    <row r="17" spans="3:25" x14ac:dyDescent="0.2">
+      <c r="E17" s="13"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+    </row>
+    <row r="18" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C18" s="10">
         <v>6</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="14"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
       <c r="Q18" s="5">
         <v>12</v>
       </c>
@@ -3408,42 +3407,42 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="3:25">
-      <c r="E19" s="15"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
-    </row>
-    <row r="20" spans="3:25">
+    <row r="19" spans="3:25" x14ac:dyDescent="0.2">
+      <c r="E19" s="13"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+    </row>
+    <row r="20" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C20" s="10">
         <v>7</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
       <c r="J20" s="11">
         <v>18</v>
       </c>
       <c r="K20" s="11">
         <v>14</v>
       </c>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="14"/>
-      <c r="P20" s="14"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
       <c r="Q20" s="5">
         <v>12</v>
       </c>
@@ -3472,49 +3471,49 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="3:25">
-      <c r="E21" s="15"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
+    <row r="21" spans="3:25" x14ac:dyDescent="0.2">
+      <c r="E21" s="13"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
       <c r="J21" s="10" t="s">
         <v>73</v>
       </c>
       <c r="K21" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="L21" s="14"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="14"/>
-      <c r="P21" s="14"/>
-    </row>
-    <row r="22" spans="3:25">
-      <c r="E22" s="15"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
-      <c r="P22" s="14"/>
-    </row>
-    <row r="23" spans="3:25">
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+    </row>
+    <row r="22" spans="3:25" x14ac:dyDescent="0.2">
+      <c r="E22" s="13"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+    </row>
+    <row r="23" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C23" s="10">
         <v>8</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
       <c r="Q23" s="5">
         <v>12</v>
       </c>
@@ -3543,28 +3542,28 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="3:25">
-      <c r="E24" s="15"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-      <c r="K24" s="14"/>
-    </row>
-    <row r="25" spans="3:25">
+    <row r="24" spans="3:25" x14ac:dyDescent="0.2">
+      <c r="E24" s="13"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+    </row>
+    <row r="25" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C25" s="10">
         <v>9</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="E25" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-      <c r="K25" s="14"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
       <c r="Q25" s="5">
         <v>12</v>
       </c>
@@ -3593,11 +3592,11 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="3:25">
+    <row r="27" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C27" s="10">
         <v>10</v>
       </c>
-      <c r="E27" s="16" t="s">
+      <c r="E27" s="14" t="s">
         <v>74</v>
       </c>
       <c r="L27" s="11">
@@ -3640,7 +3639,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="3:25">
+    <row r="28" spans="3:25" x14ac:dyDescent="0.2">
       <c r="L28" s="10" t="s">
         <v>70</v>
       </c>
@@ -3651,11 +3650,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="3:25">
+    <row r="30" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C30" s="10">
         <v>11</v>
       </c>
-      <c r="E30" s="16" t="s">
+      <c r="E30" s="14" t="s">
         <v>74</v>
       </c>
       <c r="L30" s="11">
@@ -3692,7 +3691,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="3:25">
+    <row r="31" spans="3:25" x14ac:dyDescent="0.2">
       <c r="L31" s="10" t="s">
         <v>73</v>
       </c>
@@ -3700,11 +3699,11 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="3:25">
+    <row r="33" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C33" s="10">
         <v>12</v>
       </c>
-      <c r="E33" s="16" t="s">
+      <c r="E33" s="14" t="s">
         <v>79</v>
       </c>
       <c r="Q33" s="5">
@@ -3735,38 +3734,38 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="3:25">
-      <c r="E34" s="15"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
-      <c r="K34" s="14"/>
-      <c r="P34" s="14"/>
-    </row>
-    <row r="35" spans="3:25">
+    <row r="34" spans="3:25" x14ac:dyDescent="0.2">
+      <c r="E34" s="13"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="P34" s="12"/>
+    </row>
+    <row r="35" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C35" s="10">
         <v>13</v>
       </c>
-      <c r="E35" s="16" t="s">
+      <c r="E35" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-      <c r="K35" s="14"/>
-      <c r="L35" s="14"/>
-      <c r="M35" s="14"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="12"/>
       <c r="N35" s="11">
         <v>13</v>
       </c>
       <c r="O35" s="11">
         <v>16</v>
       </c>
-      <c r="P35" s="14"/>
+      <c r="P35" s="12"/>
       <c r="Q35" s="5">
         <v>12</v>
       </c>
@@ -3795,39 +3794,39 @@
         <v>69</v>
       </c>
     </row>
-    <row r="36" spans="3:25">
-      <c r="E36" s="15"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
-      <c r="K36" s="14"/>
-      <c r="N36" s="14" t="s">
+    <row r="36" spans="3:25" x14ac:dyDescent="0.2">
+      <c r="E36" s="13"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
+      <c r="N36" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="O36" s="14" t="s">
+      <c r="O36" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="P36" s="14"/>
-    </row>
-    <row r="37" spans="3:25">
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
-      <c r="O37" s="14"/>
-      <c r="P37" s="14"/>
-    </row>
-    <row r="38" spans="3:25">
+      <c r="P36" s="12"/>
+    </row>
+    <row r="37" spans="3:25" x14ac:dyDescent="0.2">
+      <c r="L37" s="12"/>
+      <c r="M37" s="12"/>
+      <c r="N37" s="12"/>
+      <c r="O37" s="12"/>
+      <c r="P37" s="12"/>
+    </row>
+    <row r="38" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C38" s="10">
         <v>14</v>
       </c>
-      <c r="E38" s="16" t="s">
+      <c r="E38" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="L38" s="14"/>
-      <c r="M38" s="14"/>
-      <c r="P38" s="14"/>
+      <c r="L38" s="12"/>
+      <c r="M38" s="12"/>
+      <c r="P38" s="12"/>
       <c r="Q38" s="5">
         <v>12</v>
       </c>
@@ -3856,18 +3855,18 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="3:25">
-      <c r="L39" s="14"/>
-      <c r="M39" s="14"/>
-      <c r="N39" s="14"/>
-      <c r="O39" s="14"/>
-      <c r="P39" s="14"/>
-    </row>
-    <row r="40" spans="3:25">
+    <row r="39" spans="3:25" x14ac:dyDescent="0.2">
+      <c r="L39" s="12"/>
+      <c r="M39" s="12"/>
+      <c r="N39" s="12"/>
+      <c r="O39" s="12"/>
+      <c r="P39" s="12"/>
+    </row>
+    <row r="40" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C40" s="10">
         <v>15</v>
       </c>
-      <c r="E40" s="16" t="s">
+      <c r="E40" s="14" t="s">
         <v>81</v>
       </c>
       <c r="Q40" s="5">
@@ -3898,11 +3897,11 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="3:25">
+    <row r="42" spans="3:25" x14ac:dyDescent="0.2">
       <c r="C42" s="10">
         <v>16</v>
       </c>
-      <c r="E42" s="16" t="s">
+      <c r="E42" s="14" t="s">
         <v>82</v>
       </c>
       <c r="Q42" s="5">

</xml_diff>